<commit_message>
Added CaseNotes.pdf output if you add -c
</commit_message>
<xml_diff>
--- a/ForensicCasesExample.xlsx
+++ b/ForensicCasesExample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="141">
   <si>
     <t xml:space="preserve">CaseNumber</t>
   </si>
@@ -124,13 +124,52 @@
     <t xml:space="preserve">Report</t>
   </si>
   <si>
-    <t xml:space="preserve">..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationOfCaseFile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attachment</t>
+    <t xml:space="preserve">seizureAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seizureRoom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seizureStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seizedBy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exhibitType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shutdownMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shutdownTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biosTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timezone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adminUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adminPwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailPwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ip</t>
   </si>
   <si>
     <t xml:space="preserve">1931-172</t>
@@ -175,7 +214,7 @@
     <t xml:space="preserve">This was from Al Copone's phone and he gave 201711 as the pincode. This phone contained 176 instant messages between AlCopne@gmail.com and 16185551211 (James). There were message between Al Copne and his accountant.</t>
   </si>
   <si>
-    <t xml:space="preserve">On July 28, 1931, Sherlock Holmes attended the warrant at the 7244 Prairie Avenue, Illinois.</t>
+    <t xml:space="preserve">On July 28, 1931, Sherlock Holmes attended the warrant at the 7244 Prairie Avenue, Chicago Illinois.</t>
   </si>
   <si>
     <t xml:space="preserve">iOS 14.8.1</t>
@@ -193,6 +232,39 @@
     <t xml:space="preserve">Illegal Money</t>
   </si>
   <si>
+    <t xml:space="preserve">7244 Prairie Avenue, Chicago Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walt Whitman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlCopne@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
@@ -211,6 +283,18 @@
     <t xml:space="preserve">Android 11</t>
   </si>
   <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qwerty1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bugsy123@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">9</t>
   </si>
   <si>
@@ -238,6 +322,21 @@
     <t xml:space="preserve">FTK 7.5.1.127</t>
   </si>
   <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
@@ -256,6 +355,15 @@
     <t xml:space="preserve">N</t>
   </si>
   <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thugLife1234</t>
+  </si>
+  <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
@@ -280,6 +388,15 @@
     <t xml:space="preserve">FTK 7.5.2.173</t>
   </si>
   <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desktop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topOfTheWorld1</t>
+  </si>
+  <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
@@ -301,6 +418,12 @@
     <t xml:space="preserve">Windows 3.11</t>
   </si>
   <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blahblahblah</t>
+  </si>
+  <si>
     <t xml:space="preserve">13</t>
   </si>
   <si>
@@ -311,6 +434,15 @@
   </si>
   <si>
     <t xml:space="preserve">G:\Cases\1931-173-2-11_AlCapone\1931-173-2-11_Ex13_AlCapone\Image\UFED Apple iPad Air 1931_07_31 (001)\EvidenceCollection.ufdx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tacoSalad1234</t>
   </si>
 </sst>
 </file>
@@ -323,7 +455,7 @@
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -361,6 +493,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -418,7 +556,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,11 +581,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,6 +594,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,17 +682,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK1048576"/>
+  <dimension ref="A1:AX1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -581,9 +723,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="0" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="8.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="7.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="10.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="5.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="9.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="2.96"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -653,7 +808,7 @@
       <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="4" t="s">
@@ -665,13 +820,13 @@
       <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="4" t="s">
@@ -689,595 +844,931 @@
       <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="6" t="s">
         <v>36</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>13125551212</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="K2" s="8" t="n">
         <v>11535.7423611111</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="8" t="n">
         <v>11535.4916666667</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="W2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y2" s="8" t="n">
+        <v>11532.6631944444</v>
+      </c>
+      <c r="Z2" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA2" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="X2" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y2" s="9" t="n">
-        <v>11532.6631944444</v>
-      </c>
-      <c r="Z2" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA2" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="AD2" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO2" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP2" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ2" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW2" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>13124567890</v>
       </c>
-      <c r="K3" s="9" t="n">
+      <c r="K3" s="8" t="n">
         <v>11534.36875</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="W3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y3" s="8" t="n">
+        <v>11532.6631944444</v>
+      </c>
+      <c r="Z3" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA3" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y3" s="9" t="n">
-        <v>11532.6631944444</v>
-      </c>
-      <c r="Z3" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA3" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="AD3" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO3" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP3" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ3" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS3" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW3" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" s="9" t="n">
+        <v>93</v>
+      </c>
+      <c r="K4" s="8" t="n">
         <v>11532.8629050926</v>
       </c>
-      <c r="L4" s="9" t="n">
+      <c r="L4" s="8" t="n">
         <v>11532.9305902778</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="N4" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="V4" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="0" t="s">
+      <c r="W4" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="X4" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y4" s="8" t="n">
+        <v>11332.6631944444</v>
+      </c>
+      <c r="Z4" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA4" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD4" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="AH4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI4" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="U4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="X4" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y4" s="9" t="n">
-        <v>11332.6631944444</v>
-      </c>
-      <c r="Z4" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA4" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH4" s="0" t="s">
-        <v>54</v>
+      <c r="AJ4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK4" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO4" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP4" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ4" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT4" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW4" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>123456789</v>
       </c>
-      <c r="K5" s="9" t="n">
+      <c r="K5" s="8" t="n">
         <v>11534.3972222222</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="V5" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y5" s="8" t="n">
+        <v>11332.6631944444</v>
+      </c>
+      <c r="Z5" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA5" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ5" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AN5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO5" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP5" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ5" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR5" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS5" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="W5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="X5" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y5" s="9" t="n">
-        <v>11332.6631944444</v>
-      </c>
-      <c r="Z5" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA5" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB5" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH5" s="0" t="s">
-        <v>54</v>
+      <c r="AT5" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AW5" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="K6" s="9" t="n">
+        <v>116</v>
+      </c>
+      <c r="K6" s="8" t="n">
         <v>11532.806400463</v>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="8" t="n">
         <v>11532.8181944444</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="N6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="V6" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="O6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="V6" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="W6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X6" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y6" s="8" t="n">
+        <v>11332.6631944444</v>
+      </c>
+      <c r="Z6" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA6" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="X6" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y6" s="9" t="n">
-        <v>11332.6631944444</v>
-      </c>
-      <c r="Z6" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA6" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB6" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="AD6" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="AH6" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN6" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO6" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP6" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ6" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT6" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW6" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <v>11534.8638888889</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>11534.9827314815</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X7" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y7" s="8" t="n">
+        <v>11332.6631944444</v>
+      </c>
+      <c r="Z7" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA7" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK7" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN7" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="AO7" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP7" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ7" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR7" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="9" t="n">
-        <v>11534.8638888889</v>
-      </c>
-      <c r="L7" s="9" t="n">
-        <v>11534.9827314815</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="U7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="X7" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y7" s="9" t="n">
-        <v>11332.6631944444</v>
-      </c>
-      <c r="Z7" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA7" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD7" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH7" s="0" t="s">
-        <v>54</v>
+      <c r="AS7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT7" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU7" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="K8" s="9" t="n">
+        <v>136</v>
+      </c>
+      <c r="K8" s="8" t="n">
         <v>11535.4798611111</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="V8" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X8" s="9" t="n">
+        <v>11328</v>
+      </c>
+      <c r="Y8" s="8" t="n">
+        <v>11332.6631944444</v>
+      </c>
+      <c r="Z8" s="9" t="n">
+        <v>11536</v>
+      </c>
+      <c r="AA8" s="8" t="n">
+        <v>11537.4993055556</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL8" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM8" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO8" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AP8" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AQ8" s="10" t="n">
+        <v>11328.6458333333</v>
+      </c>
+      <c r="AR8" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS8" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="W8" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="X8" s="10" t="n">
-        <v>11328</v>
-      </c>
-      <c r="Y8" s="9" t="n">
-        <v>11332.6631944444</v>
-      </c>
-      <c r="Z8" s="10" t="n">
-        <v>11536</v>
-      </c>
-      <c r="AA8" s="9" t="n">
-        <v>11537.4993055556</v>
-      </c>
-      <c r="AB8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD8" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH8" s="0" t="s">
-        <v>54</v>
+      <c r="AT8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU8" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="AW8" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1309,6 +1800,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AV3" r:id="rId1" display="Bugsy123@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
updated examples, templates and more
</commit_message>
<xml_diff>
--- a/ForensicCasesExample.xlsx
+++ b/ForensicCasesExample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="161">
   <si>
     <t xml:space="preserve">caseNumber</t>
   </si>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">vaultCaseNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">vaultItem</t>
+    <t xml:space="preserve">qrCode</t>
   </si>
   <si>
     <t xml:space="preserve">vaultTotal</t>
@@ -325,9 +325,6 @@
     <t xml:space="preserve">a94a8fe5ccb19ba61c4c0873d391e987982fbbd3</t>
   </si>
   <si>
-    <t xml:space="preserve">na</t>
-  </si>
-  <si>
     <t xml:space="preserve">07/31/31 05:49 PM</t>
   </si>
   <si>
@@ -358,7 +355,10 @@
     <t xml:space="preserve">Illegal Money</t>
   </si>
   <si>
-    <t xml:space="preserve">blah</t>
+    <t xml:space="preserve">referred to AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-172_1</t>
   </si>
   <si>
     <t xml:space="preserve"> Video clips range from 5/22/1931 at 19:47 to 7/28/1931 at 10:31. Channel 1 shows the kitchen. Channel 2 is behind the bar. Channel 3 is in the kitchen sink area. Channel 4 is over the front register. Channel 5, 6, 7 and 8 have no signal. Screenshots of each working camera were taken. If additional image or video or captures are needed they can be acquired up until we return the DVR.</t>
@@ -415,7 +415,7 @@
     <t xml:space="preserve">low</t>
   </si>
   <si>
-    <t xml:space="preserve">example</t>
+    <t xml:space="preserve">1931-172_9</t>
   </si>
   <si>
     <t xml:space="preserve">This was from Al Copone's car. He used Apple Car play to sync up with his phone.</t>
@@ -454,6 +454,9 @@
     <t xml:space="preserve">G:\Cases\1931-173-2-11_AlCapone\1931-173-2-11_Ex1_AlCapone\Image\image.e01</t>
   </si>
   <si>
+    <t xml:space="preserve">1931-172_14</t>
+  </si>
+  <si>
     <t xml:space="preserve">This was from Al Copone's house. He used quicken and Turbo Tax.</t>
   </si>
   <si>
@@ -490,10 +493,16 @@
     <t xml:space="preserve">FTK 7.5.1.127</t>
   </si>
   <si>
+    <t xml:space="preserve">Arsenal Image Mounter 3.9.223</t>
+  </si>
+  <si>
     <t xml:space="preserve">G:\Cases\1931-173-2-11_AlCapone\1931-173-2-11_Ex4_AlCapone\Image\Ex4.e01</t>
   </si>
   <si>
     <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-172_15</t>
   </si>
 </sst>
 </file>
@@ -814,14 +823,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17"/>
@@ -836,10 +845,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.85"/>
@@ -850,9 +859,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="12.86"/>
@@ -862,23 +871,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="41.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="42.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="45" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="45" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="32.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="132.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="53.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="10.99"/>
   </cols>
@@ -1210,53 +1219,51 @@
       <c r="AR2" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="AS2" s="16" t="s">
+      <c r="AS2" s="16"/>
+      <c r="AT2" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="AT2" s="0" t="s">
+      <c r="AU2" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="AU2" s="0" t="s">
+      <c r="AY2" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="AY2" s="0" t="s">
+      <c r="AZ2" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="AZ2" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="BA2" s="0" t="s">
+      <c r="BB2" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="BB2" s="0" t="s">
+      <c r="BC2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="BC2" s="14" t="s">
+      <c r="BD2" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="BD2" s="14" t="s">
+      <c r="BE2" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="BE2" s="14" t="s">
+      <c r="BG2" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="BG2" s="0" t="s">
+      <c r="BH2" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="BH2" s="0" t="s">
+      <c r="BI2" s="16" t="s">
         <v>111</v>
       </c>
       <c r="BJ2" s="0" t="n">
         <v>555</v>
       </c>
       <c r="BK2" s="0" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="BL2" s="0" t="n">
         <v>12</v>
-      </c>
-      <c r="BM2" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,12 +1306,6 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q3" s="0" t="s">
         <v>117</v>
       </c>
       <c r="R3" s="0" t="s">
@@ -1395,7 +1396,7 @@
       <c r="BB3" s="18"/>
       <c r="BC3" s="18"/>
       <c r="BD3" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BE3" s="18" t="s">
         <v>129</v>
@@ -1405,28 +1406,28 @@
         <v>130</v>
       </c>
       <c r="BH3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="BI3" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="BI3" s="18"/>
       <c r="BJ3" s="0" t="n">
         <v>555</v>
       </c>
-      <c r="BK3" s="17" t="n">
-        <v>9</v>
+      <c r="BK3" s="0" t="s">
+        <v>131</v>
       </c>
       <c r="BL3" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="BM3" s="18" t="s">
-        <v>131</v>
-      </c>
+      <c r="BM3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>67</v>
@@ -1537,12 +1538,7 @@
       <c r="AP4" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="AR4" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS4" s="16" t="s">
-        <v>101</v>
-      </c>
+      <c r="AS4" s="16"/>
       <c r="AT4" s="0" t="s">
         <v>141</v>
       </c>
@@ -1550,34 +1546,34 @@
         <v>142</v>
       </c>
       <c r="BA4" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BC4" s="14" t="s">
         <v>143</v>
       </c>
       <c r="BD4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE4" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="BE4" s="14" t="s">
+      <c r="BG4" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="BG4" s="0" t="s">
+      <c r="BH4" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="BH4" s="0" t="s">
+      <c r="BI4" s="16" t="s">
         <v>111</v>
       </c>
       <c r="BJ4" s="0" t="n">
         <v>555</v>
       </c>
-      <c r="BK4" s="0" t="n">
-        <v>14</v>
+      <c r="BK4" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="BL4" s="0" t="n">
         <v>12</v>
-      </c>
-      <c r="BM4" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +1581,7 @@
         <v>65</v>
       </c>
       <c r="B5" s="22" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>67</v>
@@ -1606,32 +1602,26 @@
         <v>72</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>74</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="P5" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="R5" s="0" t="s">
         <v>81</v>
       </c>
@@ -1648,10 +1638,10 @@
         <v>81</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Y5" s="14" t="s">
         <v>85</v>
@@ -1660,7 +1650,7 @@
         <v>86</v>
       </c>
       <c r="AA5" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AB5" s="0" t="s">
         <v>88</v>
@@ -1705,19 +1695,16 @@
         <v>123</v>
       </c>
       <c r="AP5" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AQ5" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="AR5" s="0" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="AS5" s="16" t="s">
         <v>124</v>
       </c>
       <c r="AT5" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AU5" s="24" t="n">
         <v>11536.45</v>
@@ -1732,44 +1719,46 @@
         <v>1234567889</v>
       </c>
       <c r="AY5" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AZ5" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BA5" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB5" s="16"/>
+        <v>156</v>
+      </c>
+      <c r="BB5" s="16" t="s">
+        <v>157</v>
+      </c>
       <c r="BC5" s="16" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="BD5" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE5" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="BE5" s="16" t="s">
-        <v>109</v>
       </c>
       <c r="BF5" s="16"/>
       <c r="BG5" s="16" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="BH5" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="BI5" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="BI5" s="16"/>
       <c r="BJ5" s="0" t="n">
         <v>555</v>
       </c>
-      <c r="BK5" s="16" t="n">
-        <v>15</v>
+      <c r="BK5" s="0" t="s">
+        <v>160</v>
       </c>
       <c r="BL5" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="BM5" s="16" t="s">
-        <v>112</v>
-      </c>
+      <c r="BM5" s="16"/>
     </row>
   </sheetData>
   <dataValidations count="7">

</xml_diff>

<commit_message>
added agency, agencyFull, divisionFull variables so the reporting is customized to your department
</commit_message>
<xml_diff>
--- a/ForensicCasesExample.xlsx
+++ b/ForensicCasesExample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="164">
   <si>
     <t xml:space="preserve">caseNumber</t>
   </si>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">y</t>
   </si>
   <si>
-    <t xml:space="preserve">The operating system was Android 11.This was from Al Copone's phone and he gave 193104 as the pincode. This phone contained 176 instant messages between AlCopone@gmail.com and 16185551211 (James). There were message between Al Copne and his accountant.</t>
+    <t xml:space="preserve">The operating system was Android 11.This was from Al Copone's phone and he gave 193104 as the pincode. This phone contained 176 instant messages between AlCopone@gmail.com and 16185551211 (James). There were message between Al Copone and his accountant.</t>
   </si>
   <si>
     <t xml:space="preserve">On July 28, 1931, Sherlock Holmes attended the warrant at the 7244 Prairie Avenue, Chicago Illinois.</t>
@@ -382,6 +382,9 @@
     <t xml:space="preserve">d</t>
   </si>
   <si>
+    <t xml:space="preserve">finished</t>
+  </si>
+  <si>
     <t xml:space="preserve">on</t>
   </si>
   <si>
@@ -391,55 +394,58 @@
     <t xml:space="preserve">Tableau Imager 20.3.0</t>
   </si>
   <si>
+    <t xml:space="preserve">Tableau T356789iu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingston 2383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 TB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVR Examiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4th Floor Lab A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-172_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This was from Al Copone's house. He used quicken and Turbo Tax.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compaq Presario II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABESL65848Z411234 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.1.69</t>
+  </si>
+  <si>
     <t xml:space="preserve">disk to file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tableau T356789iu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kingston 2383</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 TB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DVR Examiner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4th Floor Lab A4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1931-172_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This was from Al Copone's house. He used quicken and Turbo Tax.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compaq Presario II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABESL65848Z411234 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Window 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.1.69</t>
   </si>
   <si>
     <t xml:space="preserve">6f1ed002ab5595859014ebf0951522d9</t>
@@ -818,10 +824,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.29"/>
@@ -885,7 +891,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="34.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="66" style="1" width="8.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="66" style="1" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,7 +1293,9 @@
       <c r="I3" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="K3" s="17" t="s">
         <v>114</v>
       </c>
@@ -1349,20 +1357,19 @@
       <c r="AI3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AJ3" s="17"/>
+      <c r="AJ3" s="17" t="s">
+        <v>120</v>
+      </c>
       <c r="AK3" s="1" t="s">
         <v>94</v>
       </c>
       <c r="AL3" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AM3" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AO3" s="1" t="s">
         <v>123</v>
       </c>
       <c r="AS3" s="14" t="s">
@@ -1389,14 +1396,14 @@
       <c r="BB3" s="17"/>
       <c r="BC3" s="17"/>
       <c r="BD3" s="17" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="BE3" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BF3" s="17"/>
       <c r="BG3" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BH3" s="1" t="s">
         <v>109</v>
@@ -1408,7 +1415,7 @@
         <v>555</v>
       </c>
       <c r="BK3" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BL3" s="1" t="n">
         <v>12</v>
@@ -1441,22 +1448,22 @@
         <v>72</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>74</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>117</v>
@@ -1477,10 +1484,10 @@
         <v>84</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Y4" s="14" t="s">
         <v>85</v>
@@ -1489,7 +1496,7 @@
         <v>86</v>
       </c>
       <c r="AA4" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>88</v>
@@ -1522,28 +1529,28 @@
         <v>94</v>
       </c>
       <c r="AL4" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AM4" s="14" t="s">
         <v>96</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AS4" s="14" t="s">
         <v>124</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AU4" s="21" t="n">
         <v>11536.45</v>
@@ -1564,13 +1571,13 @@
         <v>102</v>
       </c>
       <c r="BA4" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="BB4" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="BC4" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="BD4" s="14" t="s">
         <v>106</v>
@@ -1580,7 +1587,7 @@
       </c>
       <c r="BF4" s="14"/>
       <c r="BG4" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="BH4" s="1" t="s">
         <v>109</v>
@@ -1592,7 +1599,7 @@
         <v>555</v>
       </c>
       <c r="BK4" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="BL4" s="1" t="n">
         <v>12</v>
@@ -1625,22 +1632,22 @@
         <v>72</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>117</v>
@@ -1649,7 +1656,7 @@
         <v>861536030196002</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>84</v>
@@ -1667,14 +1674,14 @@
         <v>84</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="Y5" s="14"/>
       <c r="AB5" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AC5" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>90</v>
@@ -1701,29 +1708,32 @@
         <v>94</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AM5" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AN5" s="14" t="s">
-        <v>156</v>
+        <v>158</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="AS5" s="14"/>
       <c r="AT5" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AW5" s="14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="BA5" s="1" t="s">
         <v>103</v>
       </c>
       <c r="BC5" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="BD5" s="14" t="s">
         <v>106</v>
@@ -1744,7 +1754,7 @@
         <v>555</v>
       </c>
       <c r="BK5" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="BL5" s="1" t="n">
         <v>12</v>

</xml_diff>

<commit_message>
added xlsx color if report is Finalized or in Draft
</commit_message>
<xml_diff>
--- a/ForensicCasesExample.xlsx
+++ b/ForensicCasesExample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="165">
   <si>
     <t xml:space="preserve">caseNumber</t>
   </si>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">Sherlock Holmes</t>
   </si>
   <si>
-    <t xml:space="preserve">y</t>
+    <t xml:space="preserve">Finalized</t>
   </si>
   <si>
     <t xml:space="preserve">The operating system was Android 11.This was from Al Copone's phone and he gave 193104 as the pincode. This phone contained 176 instant messages between AlCopone@gmail.com and 16185551211 (James). There were message between Al Copone and his accountant.</t>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t xml:space="preserve">1931-172_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft submitted</t>
   </si>
   <si>
     <t xml:space="preserve">This was from Al Copone's car. He used Apple Car play to sync up with his phone.</t>
@@ -647,7 +650,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -708,6 +711,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -733,6 +740,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -817,17 +828,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BM5"/>
+  <dimension ref="A1:BM8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.29"/>
@@ -836,7 +847,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="48.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.57"/>
@@ -1092,7 +1103,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1104,16 +1115,16 @@
       <c r="D2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="8" t="s">
         <v>72</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1137,13 +1148,13 @@
       <c r="O2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P2" s="15" t="n">
+      <c r="P2" s="16" t="n">
         <v>3525712230449390</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="15" t="s">
         <v>81</v>
       </c>
       <c r="T2" s="1" t="s">
@@ -1155,10 +1166,10 @@
       <c r="V2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="X2" s="14" t="n">
+      <c r="X2" s="15" t="n">
         <v>193104</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="15" t="s">
         <v>85</v>
       </c>
       <c r="Z2" s="1" t="s">
@@ -1170,7 +1181,7 @@
       <c r="AB2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="15" t="s">
         <v>89</v>
       </c>
       <c r="AD2" s="1" t="s">
@@ -1182,13 +1193,13 @@
       <c r="AF2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AG2" s="14" t="s">
+      <c r="AG2" s="15" t="s">
         <v>71</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AI2" s="14" t="s">
+      <c r="AI2" s="15" t="s">
         <v>71</v>
       </c>
       <c r="AJ2" s="1" t="s">
@@ -1200,7 +1211,7 @@
       <c r="AL2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="15" t="s">
         <v>96</v>
       </c>
       <c r="AN2" s="1" t="s">
@@ -1215,7 +1226,7 @@
       <c r="AR2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AS2" s="14"/>
+      <c r="AS2" s="15"/>
       <c r="AT2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1234,13 +1245,13 @@
       <c r="BB2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BC2" s="14" t="s">
+      <c r="BC2" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="BD2" s="14" t="s">
+      <c r="BD2" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="BE2" s="14" t="s">
+      <c r="BE2" s="15" t="s">
         <v>107</v>
       </c>
       <c r="BG2" s="1" t="s">
@@ -1249,7 +1260,7 @@
       <c r="BH2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BI2" s="14" t="s">
+      <c r="BI2" s="15" t="s">
         <v>110</v>
       </c>
       <c r="BJ2" s="1" t="n">
@@ -1266,10 +1277,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="16" t="n">
+      <c r="B3" s="17" t="n">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1278,34 +1289,31 @@
       <c r="D3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="N3" s="17"/>
+      <c r="N3" s="18"/>
       <c r="O3" s="1" t="s">
         <v>117</v>
       </c>
@@ -1318,7 +1326,7 @@
       <c r="T3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U3" s="18" t="s">
         <v>118</v>
       </c>
       <c r="V3" s="1" t="s">
@@ -1330,13 +1338,13 @@
       <c r="X3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
       <c r="AB3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC3" s="14" t="s">
+      <c r="AC3" s="15" t="s">
         <v>119</v>
       </c>
       <c r="AD3" s="1" t="s">
@@ -1348,31 +1356,31 @@
       <c r="AF3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AG3" s="14" t="s">
+      <c r="AG3" s="15" t="s">
         <v>71</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AI3" s="14" t="s">
+      <c r="AI3" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AJ3" s="18" t="s">
         <v>120</v>
       </c>
       <c r="AK3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AL3" s="17" t="s">
+      <c r="AL3" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="AM3" s="19" t="s">
+      <c r="AM3" s="20" t="s">
         <v>122</v>
       </c>
       <c r="AN3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AS3" s="14" t="s">
+      <c r="AS3" s="15" t="s">
         <v>124</v>
       </c>
       <c r="AV3" s="1" t="s">
@@ -1390,25 +1398,25 @@
       <c r="AZ3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="BA3" s="17" t="s">
+      <c r="BA3" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="BB3" s="17"/>
-      <c r="BC3" s="17"/>
-      <c r="BD3" s="17" t="s">
+      <c r="BB3" s="18"/>
+      <c r="BC3" s="18"/>
+      <c r="BD3" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="BE3" s="17" t="s">
+      <c r="BE3" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="BF3" s="17"/>
-      <c r="BG3" s="17" t="s">
+      <c r="BF3" s="18"/>
+      <c r="BG3" s="18" t="s">
         <v>131</v>
       </c>
       <c r="BH3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BI3" s="14" t="s">
+      <c r="BI3" s="15" t="s">
         <v>110</v>
       </c>
       <c r="BJ3" s="1" t="n">
@@ -1420,10 +1428,10 @@
       <c r="BL3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="BM3" s="17"/>
+      <c r="BM3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -1435,34 +1443,34 @@
       <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="15" t="s">
         <v>71</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="15" t="s">
         <v>137</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -1477,7 +1485,7 @@
       <c r="T4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U4" s="14" t="s">
+      <c r="U4" s="15" t="s">
         <v>83</v>
       </c>
       <c r="V4" s="1" t="s">
@@ -1489,19 +1497,19 @@
       <c r="X4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Y4" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AA4" s="14" t="s">
+      <c r="AA4" s="15" t="s">
         <v>140</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC4" s="14" t="s">
+      <c r="AC4" s="15" t="s">
         <v>119</v>
       </c>
       <c r="AD4" s="1" t="s">
@@ -1513,25 +1521,25 @@
       <c r="AF4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AG4" s="14" t="s">
+      <c r="AG4" s="15" t="s">
         <v>71</v>
       </c>
       <c r="AH4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AI4" s="14" t="s">
+      <c r="AI4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="AJ4" s="14" t="s">
+      <c r="AJ4" s="15" t="s">
         <v>93</v>
       </c>
       <c r="AK4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AL4" s="14" t="s">
+      <c r="AL4" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="AM4" s="14" t="s">
+      <c r="AM4" s="15" t="s">
         <v>96</v>
       </c>
       <c r="AN4" s="1" t="s">
@@ -1546,13 +1554,13 @@
       <c r="AQ4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AS4" s="14" t="s">
+      <c r="AS4" s="15" t="s">
         <v>124</v>
       </c>
       <c r="AT4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AU4" s="21" t="n">
+      <c r="AU4" s="22" t="n">
         <v>11536.45</v>
       </c>
       <c r="AV4" s="1" t="s">
@@ -1570,29 +1578,29 @@
       <c r="AZ4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BA4" s="14" t="s">
+      <c r="BA4" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="BB4" s="14" t="s">
+      <c r="BB4" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="BC4" s="14" t="s">
+      <c r="BC4" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="BD4" s="14" t="s">
+      <c r="BD4" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="BE4" s="14" t="s">
+      <c r="BE4" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="BF4" s="14"/>
-      <c r="BG4" s="14" t="s">
+      <c r="BF4" s="15"/>
+      <c r="BG4" s="15" t="s">
         <v>148</v>
       </c>
       <c r="BH4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BI4" s="14" t="s">
+      <c r="BI4" s="15" t="s">
         <v>110</v>
       </c>
       <c r="BJ4" s="1" t="n">
@@ -1604,10 +1612,10 @@
       <c r="BL4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="BM4" s="14"/>
+      <c r="BM4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -1619,44 +1627,44 @@
       <c r="D5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>72</v>
+      <c r="H5" s="23" t="s">
+        <v>150</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="L5" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="M5" s="15" t="s">
         <v>154</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P5" s="22" t="n">
+      <c r="P5" s="24" t="n">
         <v>861536030196002</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>84</v>
@@ -1674,14 +1682,14 @@
         <v>84</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y5" s="14"/>
+        <v>157</v>
+      </c>
+      <c r="Y5" s="15"/>
       <c r="AB5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC5" s="14" t="s">
-        <v>157</v>
+      <c r="AC5" s="15" t="s">
+        <v>158</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>90</v>
@@ -1692,13 +1700,13 @@
       <c r="AF5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AG5" s="14" t="s">
+      <c r="AG5" s="15" t="s">
         <v>71</v>
       </c>
       <c r="AH5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AI5" s="14" t="s">
+      <c r="AI5" s="15" t="s">
         <v>71</v>
       </c>
       <c r="AJ5" s="1" t="s">
@@ -1710,35 +1718,35 @@
       <c r="AL5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AM5" s="14" t="s">
+      <c r="AM5" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="AN5" s="14" t="s">
-        <v>158</v>
+      <c r="AN5" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AS5" s="14"/>
+      <c r="AS5" s="15"/>
       <c r="AT5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="AW5" s="14" t="s">
         <v>161</v>
+      </c>
+      <c r="AW5" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="BA5" s="1" t="s">
         <v>103</v>
       </c>
       <c r="BC5" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="BD5" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD5" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="BE5" s="14" t="s">
+      <c r="BE5" s="15" t="s">
         <v>107</v>
       </c>
       <c r="BG5" s="1" t="s">
@@ -1747,18 +1755,27 @@
       <c r="BH5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BI5" s="14" t="s">
+      <c r="BI5" s="15" t="s">
         <v>110</v>
       </c>
       <c r="BJ5" s="1" t="n">
         <v>555</v>
       </c>
       <c r="BK5" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL5" s="1" t="n">
         <v>12</v>
       </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="7">

</xml_diff>

<commit_message>
sticker maker supports avery label 2x4 stickers
</commit_message>
<xml_diff>
--- a/ForensicCasesExample.xlsx
+++ b/ForensicCasesExample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="177">
   <si>
     <t xml:space="preserve">caseNumber</t>
   </si>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">This was from Al Copone's phone and he gave 193104 as the pincode. This phone contained 176 instant messages between AlCopone@gmail.com and 16185551211 (James). There were message between Al Copone and his accountant.</t>
   </si>
   <si>
-    <t xml:space="preserve">On 01/05/31 forensics examiner Sherlock Holmes attended the warrant at 7244 Prairie Avenue, Chicago Illinois.</t>
+    <t xml:space="preserve">On the evening of January 5, 1931, authorities received a tip regarding possible tax fraud by notorious gangster Al Capone. A team of investigators was dispatched to gather evidence and interview witnesses. Upon arriving at Capone's residence, at 7244 Prairie Avenue, Chicago Illinois, the investigators discovered a significant amount of financial documents and ledgers detailing the illegal activities of Capone's organization. These documents revealed that Capone had been intentionally underreporting his income and failing to pay his fair share of taxes. During questioning, several of Capone's associates admitted to being involved in the tax fraud scheme and provided further evidence of Capone's wrongdoing. Based on the evidence collected, it is clear that Capone has been engaging in tax fraud on a massive scale. He has intentionally and systematically evaded paying his fair share of taxes, thereby defrauding the government and its citizens. As a result of this investigation, authorities have issued an arrest warrant for Al Capone on charges of tax fraud.</t>
   </si>
   <si>
     <t xml:space="preserve">phone</t>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t xml:space="preserve">Video clips range from 5/22/1931 at 19:47 to 7/28/1931 at 10:31. Channel 1 shows the kitchen. Channel 2 is behind the bar. Channel 3 is in the kitchen sink area. Channel 4 is over the front register. Channel 5, 6, 7 and 8 have no signal. Screenshots of each working camera were taken. If additional image or video or captures are needed they can be acquired up until we return the DVR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 01/05/31 forensics examiner Sherlock Holmes attended the warrant at 7244 Prairie Avenue, Chicago Illinois.</t>
   </si>
   <si>
     <t xml:space="preserve">dvr</t>
@@ -828,11 +831,11 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3227,20 +3230,20 @@
         <v>120</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N3" s="0"/>
       <c r="O3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
@@ -3254,16 +3257,16 @@
         <v>83</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="V3" s="0" t="s">
         <v>85</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
@@ -3272,7 +3275,7 @@
         <v>90</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AD3" s="0" t="s">
         <v>92</v>
@@ -3297,42 +3300,42 @@
         <v>96</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AP3" s="0"/>
       <c r="AQ3" s="0"/>
       <c r="AR3" s="0"/>
       <c r="AS3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AT3" s="0"/>
       <c r="AU3" s="0"/>
       <c r="AV3" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AW3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AX3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AY3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AZ3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="BA3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BB3" s="0"/>
       <c r="BC3" s="0"/>
@@ -3340,11 +3343,11 @@
         <v>109</v>
       </c>
       <c r="BE3" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BF3" s="0"/>
       <c r="BG3" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BH3" s="0" t="s">
         <v>112</v>
@@ -3356,13 +3359,13 @@
         <v>114</v>
       </c>
       <c r="BK3" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="BL3" s="0" t="s">
         <v>116</v>
       </c>
       <c r="BM3" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BN3" s="0"/>
       <c r="BO3" s="0"/>
@@ -4329,7 +4332,7 @@
         <v>65</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>67</v>
@@ -4347,28 +4350,28 @@
         <v>71</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P4" s="0"/>
       <c r="Q4" s="0"/>
@@ -4388,10 +4391,10 @@
         <v>85</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Y4" s="0" t="s">
         <v>87</v>
@@ -4400,13 +4403,13 @@
         <v>88</v>
       </c>
       <c r="AA4" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AB4" s="0" t="s">
         <v>90</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AD4" s="0" t="s">
         <v>92</v>
@@ -4433,41 +4436,41 @@
         <v>96</v>
       </c>
       <c r="AL4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AM4" s="0" t="s">
         <v>98</v>
       </c>
       <c r="AN4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AO4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AP4" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AQ4" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AR4" s="0"/>
       <c r="AS4" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AT4" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AU4" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AV4" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AW4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AX4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AY4" s="0" t="s">
         <v>105</v>
@@ -4476,13 +4479,13 @@
         <v>105</v>
       </c>
       <c r="BA4" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="BB4" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="BC4" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="BD4" s="0" t="s">
         <v>109</v>
@@ -4492,7 +4495,7 @@
       </c>
       <c r="BF4" s="0"/>
       <c r="BG4" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="BH4" s="0" t="s">
         <v>112</v>
@@ -4504,13 +4507,13 @@
         <v>114</v>
       </c>
       <c r="BK4" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="BL4" s="0" t="s">
         <v>116</v>
       </c>
       <c r="BM4" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BN4" s="0"/>
       <c r="BO4" s="0"/>
@@ -5498,31 +5501,31 @@
         <v>72</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>85</v>
@@ -5540,7 +5543,7 @@
         <v>85</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="X5" s="0"/>
       <c r="Y5" s="0"/>
@@ -5550,7 +5553,7 @@
         <v>90</v>
       </c>
       <c r="AC5" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AD5" s="0"/>
       <c r="AE5" s="0" t="s">
@@ -5575,13 +5578,13 @@
         <v>96</v>
       </c>
       <c r="AL5" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AM5" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AN5" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AO5" s="0"/>
       <c r="AP5" s="0"/>
@@ -5589,14 +5592,14 @@
       <c r="AR5" s="0"/>
       <c r="AS5" s="0"/>
       <c r="AT5" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AU5" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AV5" s="0"/>
       <c r="AW5" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AX5" s="0"/>
       <c r="AY5" s="0"/>
@@ -5606,7 +5609,7 @@
       </c>
       <c r="BB5" s="0"/>
       <c r="BC5" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="BD5" s="0" t="s">
         <v>109</v>
@@ -5628,13 +5631,13 @@
         <v>114</v>
       </c>
       <c r="BK5" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="BL5" s="0" t="s">
         <v>116</v>
       </c>
       <c r="BM5" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BN5" s="0"/>
       <c r="BO5" s="0"/>

</xml_diff>